<commit_message>
Login error validation error message
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -395,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,10 +429,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="E3" activeCellId="0" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.1797" customWidth="1"/>
+    <col min="2" max="2" width="11.1797" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Screenshoot adn leave page
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="pim" sheetId="5" r:id="rId7"/>
+    <sheet name="testcase" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -46,18 +48,208 @@
   <si>
     <t>xyz</t>
   </si>
+  <si>
+    <t>Nagaraja</t>
+  </si>
+  <si>
+    <t>sl no</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>user id</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Login btm</t>
+  </si>
+  <si>
+    <t>clc</t>
+  </si>
+  <si>
+    <t>MainPage</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>Add Emplye</t>
+  </si>
+  <si>
+    <t>firestname</t>
+  </si>
+  <si>
+    <t>sindhu ks</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>babu</t>
+  </si>
+  <si>
+    <t>employeeid</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>Sindhu</t>
+  </si>
+  <si>
+    <t>admin321</t>
+  </si>
+  <si>
+    <t>admin3210</t>
+  </si>
+  <si>
+    <t>Sindhuu</t>
+  </si>
+  <si>
+    <t>sindhu km</t>
+  </si>
+  <si>
+    <t>baba</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>Sindhuuu</t>
+  </si>
+  <si>
+    <t>admin43210</t>
+  </si>
+  <si>
+    <t>admin53210</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>Sindhuuuu</t>
+  </si>
+  <si>
+    <t>admin63210</t>
+  </si>
+  <si>
+    <t>Sindhuuuuu</t>
+  </si>
+  <si>
+    <t>babb</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>Sindhuuuuuu</t>
+  </si>
+  <si>
+    <t>admin73210</t>
+  </si>
+  <si>
+    <t>Sindhuuuuuuu</t>
+  </si>
+  <si>
+    <t>admin83210</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>Sindhuuuuuuuu</t>
+  </si>
+  <si>
+    <t>admin93210</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>Sindhuuuuuuuuu</t>
+  </si>
+  <si>
+    <t>admin03210</t>
+  </si>
+  <si>
+    <t>Sindhuuuuuuuuuu</t>
+  </si>
+  <si>
+    <t>admin10210</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>Sindhuuuuuuuuuuu</t>
+  </si>
+  <si>
+    <t>admin20210</t>
+  </si>
+  <si>
+    <t>sindhukm</t>
+  </si>
+  <si>
+    <t>babbb</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,7 +260,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -76,12 +268,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom" horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +627,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1:B2"/>
+      <selection activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,10 +692,224 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10.9062" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="2" max="2" width="15.2695" customWidth="1"/>
+    <col min="3" max="3" width="28.2695" customWidth="1"/>
+    <col min="4" max="4" width="21.4531" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>